<commit_message>
10.05.2020 Mc Sales Details
</commit_message>
<xml_diff>
--- a/2020/Requisition/10.05.2020 Requisition of Mugdho Corporation.xlsx
+++ b/2020/Requisition/10.05.2020 Requisition of Mugdho Corporation.xlsx
@@ -1112,7 +1112,7 @@
       <pane xSplit="4" ySplit="14" topLeftCell="E15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
-      <selection pane="bottomRight" activeCell="H29" sqref="H29"/>
+      <selection pane="bottomRight" activeCell="I102" sqref="I102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21"/>
@@ -1121,8 +1121,10 @@
     <col min="2" max="2" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30" style="1" customWidth="1"/>
     <col min="4" max="4" width="26.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="29.7109375" style="1" customWidth="1"/>
-    <col min="6" max="8" width="9.140625" style="31"/>
+    <col min="5" max="5" width="27.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11" style="31" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" style="31" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" style="31" customWidth="1"/>
     <col min="9" max="9" width="11.7109375" style="31" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="31"/>
   </cols>
@@ -1633,17 +1635,19 @@
       <c r="BU9" s="19"/>
       <c r="BV9" s="19"/>
     </row>
-    <row r="10" spans="1:74" ht="15" hidden="1">
+    <row r="10" spans="1:74" ht="15">
       <c r="A10" s="5" t="s">
         <v>133</v>
       </c>
       <c r="B10" s="6">
         <v>721.8</v>
       </c>
-      <c r="C10" s="5"/>
+      <c r="C10" s="5">
+        <v>100</v>
+      </c>
       <c r="D10" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>72180</v>
       </c>
       <c r="E10" s="25" t="s">
         <v>96</v>
@@ -1788,11 +1792,11 @@
         <v>779.96</v>
       </c>
       <c r="C13" s="5">
-        <v>40</v>
+        <v>90</v>
       </c>
       <c r="D13" s="7">
         <f>C13*B13</f>
-        <v>31198.400000000001</v>
+        <v>70196.400000000009</v>
       </c>
       <c r="E13" s="25" t="s">
         <v>96</v>
@@ -1868,11 +1872,11 @@
         <v>824.06</v>
       </c>
       <c r="C18" s="5">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="D18" s="7">
         <f>C18*B18</f>
-        <v>49443.6</v>
+        <v>65924.799999999988</v>
       </c>
       <c r="E18" s="25" t="s">
         <v>96</v>
@@ -2268,11 +2272,11 @@
         <v>907.26</v>
       </c>
       <c r="C29" s="5">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D29" s="7">
         <f t="shared" si="0"/>
-        <v>70766.28</v>
+        <v>72580.800000000003</v>
       </c>
       <c r="E29" s="24" t="s">
         <v>116</v>
@@ -2611,17 +2615,19 @@
         <v>79</v>
       </c>
     </row>
-    <row r="38" spans="1:74" customFormat="1" ht="15" hidden="1">
+    <row r="38" spans="1:74" customFormat="1" ht="15">
       <c r="A38" s="5" t="s">
         <v>125</v>
       </c>
       <c r="B38" s="6">
         <v>4885.6000000000004</v>
       </c>
-      <c r="C38" s="5"/>
+      <c r="C38" s="5">
+        <v>30</v>
+      </c>
       <c r="D38" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>146568</v>
       </c>
       <c r="E38" s="24" t="s">
         <v>117</v>
@@ -2925,11 +2931,11 @@
         <v>6306.98</v>
       </c>
       <c r="C47" s="5">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="D47" s="7">
         <f t="shared" si="0"/>
-        <v>189209.4</v>
+        <v>315349</v>
       </c>
       <c r="E47" s="25" t="s">
         <v>123</v>
@@ -3055,17 +3061,19 @@
       </c>
       <c r="E53" s="5"/>
     </row>
-    <row r="54" spans="1:5" s="19" customFormat="1" ht="15" hidden="1">
+    <row r="54" spans="1:5" s="19" customFormat="1" ht="15">
       <c r="A54" s="25" t="s">
         <v>101</v>
       </c>
       <c r="B54" s="39">
         <v>1042.5999999999999</v>
       </c>
-      <c r="C54" s="25"/>
+      <c r="C54" s="25">
+        <v>30</v>
+      </c>
       <c r="D54" s="40">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>31277.999999999996</v>
       </c>
       <c r="E54" s="25" t="s">
         <v>90</v>
@@ -4061,11 +4069,11 @@
         <v>1159.8900000000001</v>
       </c>
       <c r="C94" s="5">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="D94" s="7">
         <f t="shared" si="2"/>
-        <v>69593.400000000009</v>
+        <v>115989.00000000001</v>
       </c>
       <c r="E94" s="5" t="s">
         <v>139</v>
@@ -4129,11 +4137,11 @@
         <v>1072.675</v>
       </c>
       <c r="C95" s="5">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="D95" s="7">
         <f t="shared" si="2"/>
-        <v>64360.5</v>
+        <v>107267.5</v>
       </c>
       <c r="E95" s="5" t="s">
         <v>140</v>
@@ -4197,11 +4205,11 @@
         <v>7165.02</v>
       </c>
       <c r="C96" s="5">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="D96" s="7">
         <f t="shared" si="2"/>
-        <v>214950.6</v>
+        <v>501551.4</v>
       </c>
       <c r="E96" s="25" t="s">
         <v>126</v>
@@ -4355,12 +4363,12 @@
       </c>
       <c r="B101" s="44"/>
       <c r="C101" s="27">
-        <f>SUBTOTAL(9,C7:C100)</f>
-        <v>398</v>
+        <f>SUBTOTAL(9,C10:C100)</f>
+        <v>770</v>
       </c>
       <c r="D101" s="12">
-        <f>SUBTOTAL(9,D7:D100)</f>
-        <v>722103.38</v>
+        <f>SUBTOTAL(9,D10:D100)</f>
+        <v>1531466.1</v>
       </c>
       <c r="E101" s="27"/>
       <c r="F101" s="32"/>
@@ -4592,7 +4600,7 @@
         <v>21</v>
       </c>
       <c r="C106" s="15">
-        <v>1000000</v>
+        <v>1500000</v>
       </c>
       <c r="D106" s="5" t="s">
         <v>129</v>
@@ -4746,7 +4754,7 @@
       </c>
       <c r="C110" s="16">
         <f>SUBTOTAL(9,C105:C109)</f>
-        <v>1000000</v>
+        <v>1500000</v>
       </c>
       <c r="D110" s="11"/>
       <c r="E110" s="17"/>

</xml_diff>